<commit_message>
updated in vivo data files
</commit_message>
<xml_diff>
--- a/data/stm_invivo/KP_10.5wks/KP_10.5wks_IDtoSampleType.xlsx
+++ b/data/stm_invivo/KP_10.5wks/KP_10.5wks_IDtoSampleType.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesse/Dropbox (MIT)/Bhatia Lab/_Projects/Lung Cancer/InVentiv/Batch Shipments/Lu.08/Batch I/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melodi/protease_activity_analysis/data/stm_invivo/KP_10.5wks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C2104A-FE35-004A-928F-5B8F944BBE3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE76E581-3CC7-DA49-9643-A7A543F9541F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="1860" windowWidth="26840" windowHeight="15040" xr2:uid="{BD94B0A3-C2A4-5745-A0BF-AD20916E29CE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14320" xr2:uid="{BD94B0A3-C2A4-5745-A0BF-AD20916E29CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Control</t>
   </si>
@@ -108,79 +117,13 @@
     <t>C12-2C</t>
   </si>
   <si>
-    <t>KP1-1C</t>
-  </si>
-  <si>
-    <t>KP2-1C</t>
-  </si>
-  <si>
-    <t>KP3-1C</t>
-  </si>
-  <si>
-    <t>KP4-1C</t>
-  </si>
-  <si>
-    <t>KP5-1C</t>
-  </si>
-  <si>
-    <t>KP6-1C</t>
-  </si>
-  <si>
-    <t>KP7-1C</t>
-  </si>
-  <si>
-    <t>KP8-1C</t>
-  </si>
-  <si>
-    <t>KP9-1C</t>
-  </si>
-  <si>
-    <t>KP10-1C</t>
-  </si>
-  <si>
-    <t>KP11-1C</t>
-  </si>
-  <si>
-    <t>KP12-1C</t>
-  </si>
-  <si>
-    <t>C1-1C</t>
-  </si>
-  <si>
-    <t>C2-1C</t>
-  </si>
-  <si>
-    <t>C3-1C</t>
-  </si>
-  <si>
-    <t>C4-1C</t>
-  </si>
-  <si>
-    <t>C5-1C</t>
-  </si>
-  <si>
-    <t>C6-1C</t>
-  </si>
-  <si>
-    <t>C7-1C</t>
-  </si>
-  <si>
-    <t>C8-1C</t>
-  </si>
-  <si>
-    <t>C9-1C</t>
-  </si>
-  <si>
-    <t>C10-1C</t>
-  </si>
-  <si>
-    <t>C11-1C</t>
-  </si>
-  <si>
-    <t>C12-1C</t>
-  </si>
-  <si>
     <t>KP</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>inj</t>
   </si>
 </sst>
 </file>
@@ -535,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C437C01B-3887-0842-8B88-9B9BBBDDA988}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A49" sqref="A26:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -596,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -604,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -620,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -628,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -636,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -644,7 +587,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -745,198 +688,11 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>